<commit_message>
One student showed me result of lab02.
</commit_message>
<xml_diff>
--- a/lab/lab2/lab02_Section2.xlsx
+++ b/lab/lab2/lab02_Section2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liumanni/Documents/CSE 220/cse220_2020fall/lab/lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758FD5CB-BDE9-384A-9E5E-E0ECCF65438E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4731E06-EB9A-7F41-B8FF-2C264CCDE936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{1C3543F5-1004-B644-A376-BBD6DC1ED258}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Attendance</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Attended the lab but hasn't showed me the result.</t>
+  </si>
+  <si>
+    <t>Didn't attend the lab but showed me the result.</t>
   </si>
 </sst>
 </file>
@@ -528,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C37B7-F0BE-684B-BEEA-5AEE1918F2D1}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,8 +800,11 @@
       <c r="B24" t="s">
         <v>39</v>
       </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>